<commit_message>
Simplify actions to fit new syntax
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/Night.xlsx
+++ b/scenarios/cough/processes/Night.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Nein, mein Schlaf wird nicht durch meinen Husten gestört.</t>
   </si>
   <si>
-    <t xml:space="preserve">IF ([time] == few_days) THEN (LOAD(Explanation), JUMP(Safety)) ELSE JUMP(Explanation)</t>
+    <t xml:space="preserve">IF [time] == few_days THEN LOAD(Explanation); JUMP(Safety); ELSE JUMP(Explanation)</t>
   </si>
   <si>
     <t xml:space="preserve">calmer</t>
@@ -334,7 +334,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>